<commit_message>
Mejoras, registro de usuario, manejo de ventanas, mejoras graficas
</commit_message>
<xml_diff>
--- a/Desktop/github/gestion_inventario/reporte_inventario.xlsx
+++ b/Desktop/github/gestion_inventario/reporte_inventario.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,16 +471,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Laptop HP 15</t>
+          <t>Laptop HP</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Tecnología</t>
+          <t>Electrónica</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -489,7 +489,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Distribuidora Bogotá</t>
+          <t>Proveedor A</t>
         </is>
       </c>
     </row>
@@ -499,16 +499,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Escritorio de Madera</t>
+          <t>Impresora Epson</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Muebles</t>
+          <t>Electrónica</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -517,7 +517,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Suministros Medellín</t>
+          <t>Proveedor B</t>
         </is>
       </c>
     </row>
@@ -527,109 +527,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Silla Ergonómica</t>
+          <t>arroz</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Muebles</t>
+          <t>grano</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>250000.00</t>
+          <t>1750.00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Suministros Medellín</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Monitor 24"</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Tecnología</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>9</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>800000.00</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Distribuidora Bogotá</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Impresora Multifuncional</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Tecnología</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>500000.00</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Proveedor Cali</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Arroz</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>grano</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>5</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1700.00</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Proveedor Cali</t>
+          <t>Proveedor B</t>
         </is>
       </c>
     </row>

</xml_diff>